<commit_message>
new commit for lab3
</commit_message>
<xml_diff>
--- a/Docs/lab3/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/lab3/Lab03_WBT_TCs_Form.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C526FAE9-0017-4464-9839-DF96195D1BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22152" windowHeight="13200" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="F02.TCs" sheetId="11" r:id="rId3"/>
     <sheet name="WBT-TCs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -543,7 +542,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1309,6 +1308,9 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1321,51 +1323,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1375,32 +1395,68 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1417,9 +1473,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1467,60 +1520,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1559,7 +1558,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{972C2174-200A-3C1B-CA7E-7B2CBB563DB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{972C2174-200A-3C1B-CA7E-7B2CBB563DB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1603,7 +1602,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F30BA5D2-6011-2D55-CB80-048547B4AB2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F30BA5D2-6011-2D55-CB80-048547B4AB2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1633,9 +1632,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1673,9 +1672,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1710,7 +1709,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1745,7 +1744,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1918,7 +1917,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1928,26 +1927,26 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="19.69140625" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B1" s="11"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="38" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
@@ -1957,7 +1956,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
@@ -1967,7 +1966,7 @@
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1994,7 +1993,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2009,7 +2008,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>77</v>
       </c>
@@ -2022,7 +2021,7 @@
       <c r="O9" s="26"/>
       <c r="P9" s="26"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>78</v>
       </c>
@@ -2030,7 +2029,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="36" t="s">
         <v>79</v>
       </c>
@@ -2038,15 +2037,15 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
     </row>
   </sheetData>
@@ -2059,125 +2058,125 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="17" max="17" width="10.69140625" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B1" s="11"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="44"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="B3" s="48" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="50"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="B6" s="42" t="s">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="49"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="Q6" s="42" t="s">
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="Q6" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
       <c r="I8" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="Q8" s="47" t="s">
+      <c r="Q8" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
       <c r="T8" s="33">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
       <c r="I9" s="37"/>
-      <c r="Q9" s="47" t="s">
+      <c r="Q9" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
+      <c r="R9" s="60"/>
+      <c r="S9" s="60"/>
       <c r="T9" s="33">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
       <c r="F10" s="35"/>
       <c r="G10" s="35"/>
       <c r="I10" s="51" t="s">
@@ -2189,26 +2188,26 @@
       <c r="M10" s="52"/>
       <c r="N10" s="52"/>
       <c r="O10" s="53"/>
-      <c r="Q10" s="47" t="s">
+      <c r="Q10" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="R10" s="47" t="s">
+      <c r="R10" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="47"/>
+      <c r="S10" s="60"/>
       <c r="T10" s="33">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
       <c r="I11" s="54"/>
@@ -2219,15 +2218,15 @@
       <c r="N11" s="55"/>
       <c r="O11" s="56"/>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
       <c r="F12" s="35"/>
       <c r="G12" s="35"/>
       <c r="I12" s="54"/>
@@ -2238,15 +2237,15 @@
       <c r="N12" s="55"/>
       <c r="O12" s="56"/>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
       <c r="F13" s="35"/>
       <c r="G13" s="35"/>
       <c r="I13" s="54"/>
@@ -2256,22 +2255,22 @@
       <c r="M13" s="55"/>
       <c r="N13" s="55"/>
       <c r="O13" s="56"/>
-      <c r="Q13" s="42" t="s">
+      <c r="Q13" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="R13" s="43"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="R13" s="44"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="44"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
       <c r="F14" s="35"/>
       <c r="G14" s="35"/>
       <c r="I14" s="54"/>
@@ -2282,7 +2281,7 @@
       <c r="N14" s="55"/>
       <c r="O14" s="56"/>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="I15" s="54"/>
       <c r="J15" s="55"/>
       <c r="K15" s="55"/>
@@ -2293,13 +2292,13 @@
       <c r="Q15" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="60" t="s">
+      <c r="R15" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="S15" s="61"/>
+      <c r="T15" s="61"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="I16" s="54"/>
       <c r="J16" s="55"/>
       <c r="K16" s="55"/>
@@ -2310,13 +2309,13 @@
       <c r="Q16" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="R16" s="45" t="s">
+      <c r="R16" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-    </row>
-    <row r="17" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="S16" s="46"/>
+      <c r="T16" s="46"/>
+    </row>
+    <row r="17" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I17" s="54"/>
       <c r="J17" s="55"/>
       <c r="K17" s="55"/>
@@ -2327,13 +2326,13 @@
       <c r="Q17" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="R17" s="45" t="s">
+      <c r="R17" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-    </row>
-    <row r="18" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="S17" s="46"/>
+      <c r="T17" s="46"/>
+    </row>
+    <row r="18" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I18" s="54"/>
       <c r="J18" s="55"/>
       <c r="K18" s="55"/>
@@ -2344,13 +2343,13 @@
       <c r="Q18" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="R18" s="45" t="s">
+      <c r="R18" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-    </row>
-    <row r="19" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="S18" s="46"/>
+      <c r="T18" s="46"/>
+    </row>
+    <row r="19" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I19" s="54"/>
       <c r="J19" s="55"/>
       <c r="K19" s="55"/>
@@ -2361,13 +2360,13 @@
       <c r="Q19" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="R19" s="45" t="s">
+      <c r="R19" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-    </row>
-    <row r="20" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="S19" s="46"/>
+      <c r="T19" s="46"/>
+    </row>
+    <row r="20" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I20" s="54"/>
       <c r="J20" s="55"/>
       <c r="K20" s="55"/>
@@ -2378,13 +2377,13 @@
       <c r="Q20" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="R20" s="45" t="s">
+      <c r="R20" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
-    </row>
-    <row r="21" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="S20" s="46"/>
+      <c r="T20" s="46"/>
+    </row>
+    <row r="21" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I21" s="54"/>
       <c r="J21" s="55"/>
       <c r="K21" s="55"/>
@@ -2393,11 +2392,11 @@
       <c r="N21" s="55"/>
       <c r="O21" s="56"/>
       <c r="Q21" s="34"/>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="45"/>
-    </row>
-    <row r="22" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
+      <c r="T21" s="46"/>
+    </row>
+    <row r="22" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I22" s="54"/>
       <c r="J22" s="55"/>
       <c r="K22" s="55"/>
@@ -2406,7 +2405,7 @@
       <c r="N22" s="55"/>
       <c r="O22" s="56"/>
     </row>
-    <row r="23" spans="9:20" x14ac:dyDescent="0.4">
+    <row r="23" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I23" s="54"/>
       <c r="J23" s="55"/>
       <c r="K23" s="55"/>
@@ -2415,7 +2414,7 @@
       <c r="N23" s="55"/>
       <c r="O23" s="56"/>
     </row>
-    <row r="24" spans="9:20" x14ac:dyDescent="0.4">
+    <row r="24" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I24" s="57"/>
       <c r="J24" s="58"/>
       <c r="K24" s="58"/>
@@ -2426,6 +2425,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R21:T21"/>
@@ -2442,14 +2449,6 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2458,7 +2457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
@@ -2468,116 +2467,116 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.3046875" customWidth="1"/>
-    <col min="3" max="4" width="18.23046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.23046875" customWidth="1"/>
-    <col min="7" max="7" width="11.3828125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.23046875" customWidth="1"/>
-    <col min="9" max="9" width="9.3046875" customWidth="1"/>
-    <col min="10" max="10" width="14.69140625" customWidth="1"/>
-    <col min="11" max="11" width="6.07421875" customWidth="1"/>
-    <col min="12" max="12" width="6.3828125" customWidth="1"/>
-    <col min="13" max="13" width="12.23046875" customWidth="1"/>
-    <col min="15" max="15" width="11.765625" customWidth="1"/>
-    <col min="16" max="16" width="8.765625" customWidth="1"/>
-    <col min="17" max="17" width="8.921875" customWidth="1"/>
-    <col min="21" max="21" width="9.07421875" customWidth="1"/>
-    <col min="22" max="22" width="2.23046875" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="2.07421875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.53515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="2.23046875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.07421875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" customWidth="1"/>
+    <col min="15" max="15" width="11.77734375" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" customWidth="1"/>
+    <col min="21" max="21" width="9.109375" customWidth="1"/>
+    <col min="22" max="22" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B1" s="11"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.4">
-      <c r="B3" s="69" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B3" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-    </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.4">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="49"/>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="2:28" ht="15.9" x14ac:dyDescent="0.4">
-      <c r="B6" s="70" t="s">
+    <row r="6" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="70"/>
-      <c r="U6" s="70"/>
-      <c r="V6" s="70"/>
-      <c r="W6" s="70"/>
-      <c r="X6" s="70"/>
-      <c r="Y6" s="70"/>
-      <c r="Z6" s="70"/>
-      <c r="AA6" s="70"/>
-      <c r="AB6" s="70"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.9" x14ac:dyDescent="0.4">
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="64" t="s">
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="63"/>
+      <c r="Z6" s="63"/>
+      <c r="AA6" s="63"/>
+      <c r="AB6" s="63"/>
+    </row>
+    <row r="7" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="63" t="s">
+      <c r="F7" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="63"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="65" t="s">
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="Q7" s="65"/>
-      <c r="R7" s="65"/>
-      <c r="S7" s="65"/>
-      <c r="T7" s="65"/>
-      <c r="U7" s="65"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="67"/>
       <c r="V7" s="66" t="s">
         <v>20</v>
       </c>
@@ -2588,49 +2587,49 @@
       <c r="AA7" s="66"/>
       <c r="AB7" s="66"/>
     </row>
-    <row r="8" spans="2:28" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="70"/>
-      <c r="C8" s="61" t="s">
+    <row r="8" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="63"/>
+      <c r="C8" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="64"/>
-      <c r="F8" s="63" t="s">
+      <c r="E8" s="73"/>
+      <c r="F8" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63" t="s">
+      <c r="G8" s="70"/>
+      <c r="H8" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63" t="s">
+      <c r="I8" s="70"/>
+      <c r="J8" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="63"/>
-      <c r="L8" s="63" t="s">
+      <c r="K8" s="70"/>
+      <c r="L8" s="70" t="s">
         <v>105</v>
       </c>
-      <c r="M8" s="63"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="65" t="s">
+      <c r="M8" s="70"/>
+      <c r="N8" s="70"/>
+      <c r="O8" s="70"/>
+      <c r="P8" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="Q8" s="65" t="s">
+      <c r="Q8" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="R8" s="67" t="s">
+      <c r="R8" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="S8" s="67" t="s">
+      <c r="S8" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="T8" s="67" t="s">
+      <c r="T8" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="U8" s="65"/>
+      <c r="U8" s="67"/>
       <c r="V8" s="66">
         <v>0</v>
       </c>
@@ -2653,11 +2652,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:28" ht="15.9" x14ac:dyDescent="0.4">
-      <c r="B9" s="70"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="64"/>
+    <row r="9" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="63"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="73"/>
       <c r="F9" s="12" t="s">
         <v>25</v>
       </c>
@@ -2688,12 +2687,12 @@
       <c r="O9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="68"/>
-      <c r="S9" s="68"/>
-      <c r="T9" s="68"/>
-      <c r="U9" s="65"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="67"/>
+      <c r="R9" s="72"/>
+      <c r="S9" s="72"/>
+      <c r="T9" s="72"/>
+      <c r="U9" s="67"/>
       <c r="V9" s="66"/>
       <c r="W9" s="66"/>
       <c r="X9" s="66"/>
@@ -2702,7 +2701,7 @@
       <c r="AA9" s="66"/>
       <c r="AB9" s="66"/>
     </row>
-    <row r="10" spans="2:28" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:28" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
         <v>50</v>
       </c>
@@ -2751,7 +2750,7 @@
       <c r="AA10" s="18"/>
       <c r="AB10" s="18"/>
     </row>
-    <row r="11" spans="2:28" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:28" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B11" s="13" t="s">
         <v>51</v>
       </c>
@@ -2800,7 +2799,7 @@
       <c r="AA11" s="18"/>
       <c r="AB11" s="18"/>
     </row>
-    <row r="12" spans="2:28" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="13"/>
       <c r="C12" s="39"/>
       <c r="D12" s="14"/>
@@ -2829,7 +2828,7 @@
       <c r="AA12" s="18"/>
       <c r="AB12" s="18"/>
     </row>
-    <row r="13" spans="2:28" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="14"/>
@@ -2858,7 +2857,7 @@
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
     </row>
-    <row r="14" spans="2:28" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="14"/>
@@ -2887,7 +2886,7 @@
       <c r="AA14" s="18"/>
       <c r="AB14" s="18"/>
     </row>
-    <row r="15" spans="2:28" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="14"/>
@@ -2916,11 +2915,25 @@
       <c r="AA15" s="18"/>
       <c r="AB15" s="18"/>
     </row>
-    <row r="16" spans="2:28" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:O7"/>
+    <mergeCell ref="P7:U7"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -2937,20 +2950,6 @@
     <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="V7:AB7"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:O7"/>
-    <mergeCell ref="P7:U7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2958,82 +2957,82 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="7.23046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.07421875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.23046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.07421875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.07421875" customWidth="1"/>
-    <col min="13" max="13" width="16.07421875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.3046875" customWidth="1"/>
+    <col min="10" max="10" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" s="11"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B3" s="97" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B4" s="98" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="100" t="s">
+      <c r="E4" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="100" t="s">
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="101"/>
-    </row>
-    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="99"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="109"/>
+      <c r="L4" s="80"/>
+    </row>
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="78"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="89"/>
       <c r="E5" s="2" t="s">
         <v>88</v>
       </c>
@@ -3042,8 +3041,8 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="103"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="82"/>
       <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3051,17 +3050,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="32.15" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:14" ht="31.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20">
         <v>9</v>
       </c>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="83" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="112">
+      <c r="E6" s="42">
         <v>40179</v>
       </c>
       <c r="F6" s="40">
@@ -3069,8 +3068,8 @@
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="111"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="91"/>
       <c r="K6" s="14" t="s">
         <v>100</v>
       </c>
@@ -3078,11 +3077,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="31.75" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B7" s="20">
         <v>10</v>
       </c>
-      <c r="C7" s="104"/>
+      <c r="C7" s="83"/>
       <c r="D7" s="13" t="s">
         <v>51</v>
       </c>
@@ -3094,8 +3093,8 @@
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="101"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="80"/>
       <c r="K7" s="14" t="s">
         <v>87</v>
       </c>
@@ -3103,46 +3102,46 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="20"/>
-      <c r="C8" s="104"/>
+      <c r="C8" s="83"/>
       <c r="D8" s="13"/>
       <c r="E8" s="41"/>
       <c r="F8" s="41"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="100"/>
-      <c r="J8" s="101"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="80"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="20"/>
-      <c r="C9" s="104"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="9"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="100"/>
-      <c r="J9" s="101"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="80"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
     </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
-      <c r="C10" s="105"/>
+      <c r="C10" s="84"/>
       <c r="D10" s="8"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="103"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="82"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -3155,98 +3154,104 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="2:14" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="73" t="s">
+    <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="75" t="s">
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="76"/>
-      <c r="H13" s="73" t="s">
+      <c r="G13" s="95"/>
+      <c r="H13" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="91"/>
-      <c r="M13" s="95" t="s">
+      <c r="I13" s="93"/>
+      <c r="J13" s="93"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="109"/>
+      <c r="M13" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="N13" s="96"/>
-    </row>
-    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="86" t="s">
+      <c r="N13" s="75"/>
+    </row>
+    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="82" t="s">
+      <c r="C14" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="D14" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="88" t="s">
+      <c r="E14" s="106" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="79" t="s">
+      <c r="F14" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="77" t="s">
+      <c r="G14" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="80" t="s">
+      <c r="H14" s="98" t="s">
         <v>71</v>
       </c>
-      <c r="I14" s="82" t="s">
+      <c r="I14" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="82" t="s">
+      <c r="J14" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="84" t="s">
+      <c r="K14" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="92" t="s">
+      <c r="L14" s="110" t="s">
         <v>72</v>
       </c>
-      <c r="M14" s="94" t="s">
+      <c r="M14" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="N14" s="78" t="s">
+      <c r="N14" s="86" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B15" s="87"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="85"/>
-      <c r="L15" s="93"/>
-      <c r="M15" s="86"/>
-      <c r="N15" s="79"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="105"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="101"/>
+      <c r="J15" s="101"/>
+      <c r="K15" s="103"/>
+      <c r="L15" s="111"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="97"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="26">
         <v>2</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
+      <c r="C16" s="23">
+        <v>2</v>
+      </c>
+      <c r="D16" s="23">
+        <v>0</v>
+      </c>
+      <c r="E16" s="24">
+        <v>47</v>
+      </c>
       <c r="F16" s="25"/>
       <c r="G16" s="7"/>
       <c r="H16" s="6"/>
@@ -3259,6 +3264,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
@@ -3275,21 +3295,6 @@
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3297,21 +3302,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5F472198D7887469049920058585067" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e76e8f6ca957e849a493f1baa4f4bb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c46c0853-0d59-45c6-b517-3e25eac8cdf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ddeb00cc2097713d6f56fe4f26be38f" ns2:_="">
     <xsd:import namespace="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -3455,24 +3445,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E53DB3A-2750-466D-B803-7A1FAB16D24B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3488,4 +3476,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>